<commit_message>
build mnthly report download process
</commit_message>
<xml_diff>
--- a/Performer_GenerateYearlyReport/Data/Config.xlsx
+++ b/Performer_GenerateYearlyReport/Data/Config.xlsx
@@ -1,28 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ford\Documents\UIPath\GenerateYearlyReport\Performer_GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29032C11-5105-4CFB-B0A0-933B9917CE32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA75BF0D-B24A-4744-91F3-8DEE983DA294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +139,12 @@
   </si>
   <si>
     <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>ReportsDownloadPath</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -512,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -600,7 +616,14 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1602,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>